<commit_message>
Feat : Read Data Excel
</commit_message>
<xml_diff>
--- a/files/excel/GeneralCode.xlsx
+++ b/files/excel/GeneralCode.xlsx
@@ -1,39 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\automation\RPAAutomation\files\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>General Code</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>IsEditable</t>
+  </si>
+  <si>
+    <t>A55123</t>
+  </si>
+  <si>
+    <t>Example Item 1</t>
+  </si>
+  <si>
+    <t>DXF456</t>
+  </si>
+  <si>
+    <t>Example Item 2</t>
+  </si>
+  <si>
+    <t>GHG789</t>
+  </si>
+  <si>
+    <t>Example Item 3</t>
+  </si>
+  <si>
+    <t>JKS012</t>
+  </si>
+  <si>
+    <t>Example Item 4</t>
+  </si>
+  <si>
+    <t>Example Item 6</t>
+  </si>
+  <si>
+    <t>Example Item 7</t>
+  </si>
+  <si>
+    <t>Example Item 8</t>
+  </si>
+  <si>
+    <t>MXO723</t>
+  </si>
+  <si>
+    <t>MFO235</t>
+  </si>
+  <si>
+    <t>MHO841</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
     </font>
     <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -52,90 +118,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" headerRowCount="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" totalsRowShown="0">
   <autoFilter ref="A2:D3"/>
   <tableColumns count="4">
     <tableColumn id="1" name="No"/>
@@ -431,176 +438,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E25"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="14.7109375" bestFit="1" customWidth="1" style="3" min="1" max="3"/>
-    <col width="14.7109375" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-    <col width="14.7109375" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col min="1" max="5" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>General Code</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>IsEditable</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A55123</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Example Item 1</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>DXF456</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Example Item 2</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GHG789</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Example Item 3</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>JKS012</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Example Item 4</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>MXO345</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Example Item 5</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
         <v>-1</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>MFO345</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Example Item 5</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
         <v>-1</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>MHO345</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Example Item 5</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
         <v>-1</v>
       </c>
     </row>
@@ -610,7 +576,7 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <tableParts count="1">
-    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>